<commit_message>
implement null hypothesis-based feature selection
</commit_message>
<xml_diff>
--- a/docs/Model Log.xlsx
+++ b/docs/Model Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>时间</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>rank</t>
-  </si>
-  <si>
-    <t>具体分数</t>
   </si>
   <si>
     <t>耗时</t>
@@ -63,18 +60,56 @@
 5. 模型ensemble</t>
   </si>
   <si>
-    <t xml:space="preserve">A:0.0306 
-B:-0.4867 
-C:0.0917 
-D:0.1334 
-E:0.4383 </t>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. 表格merge: HASH_MAX = 200 WINDOW_SIZE = 5; 
+2. categorical hash: frequency encoding; 
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>null hypothesis-based feature selection</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+4. 数据平衡：下采样；
+5. 模型ensemble</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +129,14 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,7 +461,7 @@
     <col min="3" max="3" width="63.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,51 +475,87 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43607</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43609</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3">
         <v>38</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
+      <c r="E3" s="2">
+        <v>0.69599999999999995</v>
       </c>
       <c r="F3">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="H3">
+        <v>0.74199999999999999</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="J3">
         <v>4174</v>
       </c>
+    </row>
+    <row r="4" spans="1:10" ht="80" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43610</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
merge weekly progress md
</commit_message>
<xml_diff>
--- a/docs/Model Log.xlsx
+++ b/docs/Model Log.xlsx
@@ -486,7 +486,7 @@
   <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,7 +604,13 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D5">
+        <v>87</v>
+      </c>
       <c r="E5" s="2"/>
+      <c r="J5">
+        <v>4416</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implement one process method for multi-value category
</commit_message>
<xml_diff>
--- a/docs/Model Log.xlsx
+++ b/docs/Model Log.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>时间</t>
   </si>
@@ -137,6 +137,40 @@
 5. 数据平衡：下采样；
 6. 模型ensemble</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. 表格merge: HASH_MAX = 200 WINDOW_SIZE = 5; 
+2. categorical hash: factorization; 
+3. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>feature selection simple</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+4. 模型ensemble</t>
+    </r>
+  </si>
+  <si>
+    <t>1. 表格merge: HASH_MAX = 200 WINDOW_SIZE = 5; 
+2. categorical hash: factorization
+3. 模型ensemble</t>
   </si>
 </sst>
 </file>
@@ -483,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,6 +646,31 @@
         <v>4416</v>
       </c>
     </row>
+    <row r="6" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43611</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43611</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>